<commit_message>
WHS price code added
</commit_message>
<xml_diff>
--- a/Valid_ImportTemplate/Area RRP 2022 Spring-Summer.xlsx
+++ b/Valid_ImportTemplate/Area RRP 2022 Spring-Summer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Article Number</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>75</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>66</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
TestNg XML and Retry and Extent Report added
</commit_message>
<xml_diff>
--- a/Valid_ImportTemplate/Area RRP 2022 Spring-Summer.xlsx
+++ b/Valid_ImportTemplate/Area RRP 2022 Spring-Summer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Article Number</t>
   </si>
@@ -80,6 +80,39 @@
   </si>
   <si>
     <t>66</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>76</t>
   </si>
 </sst>
 </file>
@@ -445,7 +478,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>